<commit_message>
Update from Chapter 12 and 13
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue - Chapter 12.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue - Chapter 12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515116ED-085C-4F40-846F-D08A8E266E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0902B6-EFE7-4631-B2BA-985805663CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
   <si>
     <t>Feature</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Sales Document</t>
   </si>
   <si>
-    <t>LookupValue</t>
-  </si>
-  <si>
     <t>Warehouse Shipment</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>Posting</t>
-  </si>
-  <si>
-    <t>Lookup Value</t>
   </si>
   <si>
     <t>ATDD.TestScriptor Format</t>
@@ -412,6 +406,69 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -507,69 +564,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -584,28 +578,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M40" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M40" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:M40" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="15">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="13">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -911,7 +905,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -944,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -965,7 +959,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>10</v>
@@ -976,7 +970,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -984,7 +978,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
       <c r="H2" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="16" t="str">
@@ -1006,7 +1000,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>17</v>
@@ -1016,7 +1010,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="21"/>
@@ -1042,7 +1036,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -1054,7 +1048,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I4" s="13">
         <v>100</v>
@@ -1077,7 +1071,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1089,7 +1083,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I5" s="13">
         <v>100</v>
@@ -1112,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -1124,7 +1118,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" s="13">
         <v>100</v>
@@ -1147,7 +1141,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>17</v>
@@ -1155,7 +1149,7 @@
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="21"/>
@@ -1181,7 +1175,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -1190,7 +1184,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I8" s="13">
         <v>101</v>
@@ -1213,7 +1207,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -1222,7 +1216,7 @@
         <v>14</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I9" s="13">
         <v>101</v>
@@ -1245,7 +1239,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1254,7 +1248,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I10" s="13">
         <v>101</v>
@@ -1274,20 +1268,20 @@
     </row>
     <row r="11" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>19</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="21"/>
@@ -1310,13 +1304,13 @@
     </row>
     <row r="12" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>16</v>
@@ -1325,7 +1319,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I12" s="13">
         <v>102</v>
@@ -1345,13 +1339,13 @@
     </row>
     <row r="13" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>16</v>
@@ -1360,7 +1354,7 @@
         <v>14</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I13" s="13">
         <v>102</v>
@@ -1380,13 +1374,13 @@
     </row>
     <row r="14" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>16</v>
@@ -1395,7 +1389,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I14" s="13">
         <v>102</v>
@@ -1415,18 +1409,18 @@
     </row>
     <row r="15" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>19</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="21"/>
@@ -1449,19 +1443,19 @@
     </row>
     <row r="16" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I16" s="13">
         <v>103</v>
@@ -1481,19 +1475,19 @@
     </row>
     <row r="17" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
         <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I17" s="13">
         <v>103</v>
@@ -1513,19 +1507,19 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
         <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
       </c>
       <c r="G18" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I18" s="13">
         <v>103</v>
@@ -1548,7 +1542,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1556,7 +1550,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="5"/>
       <c r="H19" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="16" t="str">
@@ -1578,13 +1572,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="21"/>
@@ -1610,13 +1604,13 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I21" s="25">
         <v>104</v>
@@ -1639,13 +1633,13 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I22" s="25">
         <v>104</v>
@@ -1668,13 +1662,13 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I23" s="25">
         <v>104</v>
@@ -1697,13 +1691,13 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G24" t="s">
         <v>15</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I24" s="25">
         <v>104</v>
@@ -1726,13 +1720,13 @@
         <v>11</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="21"/>
@@ -1758,13 +1752,13 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s">
         <v>13</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I26" s="13">
         <v>105</v>
@@ -1787,7 +1781,7 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G27" t="s">
         <v>13</v>
@@ -1816,13 +1810,13 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I28" s="13">
         <v>105</v>
@@ -1845,13 +1839,13 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G29" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I29" s="13">
         <v>105</v>
@@ -1874,13 +1868,13 @@
         <v>11</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="21"/>
@@ -1906,13 +1900,13 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G31" t="s">
         <v>13</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I31" s="13">
         <v>106</v>
@@ -1935,7 +1929,7 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G32" t="s">
         <v>13</v>
@@ -1964,13 +1958,13 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G33" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I33" s="13">
         <v>106</v>
@@ -1993,13 +1987,13 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G34" t="s">
         <v>15</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I34" s="13">
         <v>106</v>
@@ -2022,7 +2016,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
@@ -2030,7 +2024,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="5"/>
       <c r="H35" s="31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="16" t="str">
@@ -2052,13 +2046,13 @@
         <v>11</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" s="32"/>
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G36" s="32"/>
       <c r="H36" s="35"/>
@@ -2084,13 +2078,13 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G37" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I37" s="13">
         <v>107</v>
@@ -2113,13 +2107,13 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G38" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I38" s="13">
         <v>107</v>
@@ -2142,13 +2136,13 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I39" s="13">
         <v>107</v>
@@ -2171,13 +2165,13 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G40" t="s">
         <v>15</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I40" s="13">
         <v>107</v>
@@ -2210,28 +2204,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:D1048576 D1:D34">
-    <cfRule type="cellIs" dxfId="11" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B1048576 A1:B34">
-    <cfRule type="containsBlanks" dxfId="10" priority="50">
+    <cfRule type="containsBlanks" dxfId="20" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:E1048576 E1:E34">
-    <cfRule type="cellIs" dxfId="9" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G1048576 G1:G34">
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2248,28 +2242,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B35">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="14" priority="5">
       <formula>LEN(TRIM(A35))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Rewrite of example 11 unit tests
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue - Chapter 12.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue - Chapter 12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0902B6-EFE7-4631-B2BA-985805663CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0699A838-20D2-4642-92A9-DB7326D1B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
   <si>
     <t>Feature</t>
   </si>
@@ -141,61 +141,58 @@
     <t>Missing lookup value on sales header error thrown</t>
   </si>
   <si>
-    <t>Check failure OnBeforePostSalesDocEvent subscriber</t>
-  </si>
-  <si>
     <t>Sales header with lookup value</t>
   </si>
   <si>
-    <t>Check failure OnBeforePostSourceDocumentEvent subscriber</t>
-  </si>
-  <si>
     <t>Sales header with number and lookup value</t>
   </si>
   <si>
     <t>Sales header with number and without lookup value</t>
   </si>
   <si>
-    <t>Check success OnBeforePostSourceDocumentEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check success OnBeforePostSalesDocEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</t>
-  </si>
-  <si>
-    <t>Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</t>
-  </si>
-  <si>
     <t>Warehouse shipment line</t>
   </si>
   <si>
     <t>Lookup value on warehouse shipment line is populated with lookup value of sales header</t>
   </si>
   <si>
-    <t xml:space="preserve">OnBeforeCreateShptLineFromSalesLineEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnBeforePostSalesDocEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnBeforePostSourceDocumentEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OnApplyTemplateOnBeforeCustomerModifyEvent </t>
+    <t>Check failure CheckLookupvalueExistsOnSalesHeader Sales Posting</t>
+  </si>
+  <si>
+    <t>Check success CheckLookupvalueExistsOnSalesHeader Sales Posting</t>
+  </si>
+  <si>
+    <t>Check failure CheckLookupvalueExistsOnSalesHeader Whse. Posting</t>
+  </si>
+  <si>
+    <t>Check success CheckLookupvalueExistsOnSalesHeader Whse. Posting</t>
+  </si>
+  <si>
+    <t>Check InheritLookupValueFromSalesHeader</t>
+  </si>
+  <si>
+    <t>Trigger InheritLookupValueFromSalesHeader</t>
+  </si>
+  <si>
+    <t>Trigger InheritLookupValueFromCustomer</t>
+  </si>
+  <si>
+    <t>Check InheritLookupValueFromCustomer</t>
+  </si>
+  <si>
+    <t>Trigger ApplyLookupValueFromCustomerTemplate</t>
+  </si>
+  <si>
+    <t>Check ApplyLookupValueFromCustomerTemplate</t>
+  </si>
+  <si>
+    <t>Check ApplyLookupValueFromCustomerTemplate from Contact</t>
+  </si>
+  <si>
+    <t>Trigger CheckLookupvalueExistsOnSalesHeader Sales Posting</t>
+  </si>
+  <si>
+    <t>Trigger CheckLookupvalueExistsOnSalesHeader Whse. Posting</t>
   </si>
 </sst>
 </file>
@@ -904,9 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -995,7 +990,7 @@
       </c>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>11</v>
       </c>
@@ -1010,7 +1005,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="21"/>
@@ -1019,15 +1014,15 @@
       </c>
       <c r="J3" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0100] Check failure OnBeforePostSalesDocEvent subscriber</v>
+        <v>[SCENARIO #0100] Check failure CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="K3" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0100] Check failure OnBeforePostSalesDocEvent subscriber</v>
+        <v>//[SCENARIO #0100] Check failure CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="L3" s="29" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0100 'Check failure OnBeforePostSalesDocEvent subscriber' {</v>
+        <v>Scenario 0100 'Check failure CheckLookupvalueExistsOnSalesHeader Sales Posting' {</v>
       </c>
       <c r="M3" s="21"/>
     </row>
@@ -1066,7 +1061,7 @@
         <v>Given 'Sales header without lookup value'</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1083,22 +1078,22 @@
         <v>14</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I5" s="13">
         <v>100</v>
       </c>
       <c r="J5" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSalesDocEvent </v>
+        <v>[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="K5" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSalesDocEvent </v>
+        <v>//[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="L5" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSalesDocEvent '</v>
+        <v>When 'Trigger CheckLookupvalueExistsOnSalesHeader Sales Posting'</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1136,7 +1131,7 @@
         <v>Then 'Missing lookup value on sales header error thrown' }</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>11</v>
       </c>
@@ -1158,15 +1153,15 @@
       </c>
       <c r="J7" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0101] Check success OnBeforePostSalesDocEvent subscriber</v>
+        <v>[SCENARIO #0101] Check success CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="K7" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0101] Check success OnBeforePostSalesDocEvent subscriber</v>
+        <v>//[SCENARIO #0101] Check success CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="L7" s="29" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0101 'Check success OnBeforePostSalesDocEvent subscriber' {</v>
+        <v>Scenario 0101 'Check success CheckLookupvalueExistsOnSalesHeader Sales Posting' {</v>
       </c>
       <c r="M7" s="21"/>
     </row>
@@ -1184,7 +1179,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="13">
         <v>101</v>
@@ -1202,7 +1197,7 @@
         <v>Given 'Sales header with lookup value'</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1216,22 +1211,22 @@
         <v>14</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I9" s="13">
         <v>101</v>
       </c>
       <c r="J9" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSalesDocEvent </v>
+        <v>[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="K9" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSalesDocEvent </v>
+        <v>//[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Sales Posting</v>
       </c>
       <c r="L9" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSalesDocEvent '</v>
+        <v>When 'Trigger CheckLookupvalueExistsOnSalesHeader Sales Posting'</v>
       </c>
     </row>
     <row r="10" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1266,7 +1261,7 @@
         <v>Then 'No error thrown' }</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>11</v>
       </c>
@@ -1281,7 +1276,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="21"/>
@@ -1290,15 +1285,15 @@
       </c>
       <c r="J11" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0102] Check failure OnBeforePostSourceDocumentEvent subscriber</v>
+        <v>[SCENARIO #0102] Check failure CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="K11" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0102] Check failure OnBeforePostSourceDocumentEvent subscriber</v>
+        <v>//[SCENARIO #0102] Check failure CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="L11" s="29" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0102 'Check failure OnBeforePostSourceDocumentEvent subscriber' {</v>
+        <v>Scenario 0102 'Check failure CheckLookupvalueExistsOnSalesHeader Whse. Posting' {</v>
       </c>
       <c r="M11" s="21"/>
     </row>
@@ -1319,7 +1314,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I12" s="13">
         <v>102</v>
@@ -1337,7 +1332,7 @@
         <v>Given 'Sales header with number and without lookup value'</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1354,22 +1349,22 @@
         <v>14</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I13" s="13">
         <v>102</v>
       </c>
       <c r="J13" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSourceDocumentEvent </v>
+        <v>[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="K13" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSourceDocumentEvent </v>
+        <v>//[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="L13" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSourceDocumentEvent '</v>
+        <v>When 'Trigger CheckLookupvalueExistsOnSalesHeader Whse. Posting'</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1407,7 +1402,7 @@
         <v>Then 'Missing lookup value on sales header error thrown' }</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>11</v>
       </c>
@@ -1420,7 +1415,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="21"/>
@@ -1429,15 +1424,15 @@
       </c>
       <c r="J15" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0103] Check success OnBeforePostSourceDocumentEvent subscriber</v>
+        <v>[SCENARIO #0103] Check success CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="K15" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0103] Check success OnBeforePostSourceDocumentEvent subscriber</v>
+        <v>//[SCENARIO #0103] Check success CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="L15" s="29" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0103 'Check success OnBeforePostSourceDocumentEvent subscriber' {</v>
+        <v>Scenario 0103 'Check success CheckLookupvalueExistsOnSalesHeader Whse. Posting' {</v>
       </c>
       <c r="M15" s="21"/>
     </row>
@@ -1455,7 +1450,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I16" s="13">
         <v>103</v>
@@ -1473,7 +1468,7 @@
         <v>Given 'Sales header with number and lookup value'</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1487,22 +1482,22 @@
         <v>14</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I17" s="13">
         <v>103</v>
       </c>
       <c r="J17" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforePostSourceDocumentEvent </v>
+        <v>[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="K17" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforePostSourceDocumentEvent </v>
+        <v>//[WHEN] Trigger CheckLookupvalueExistsOnSalesHeader Whse. Posting</v>
       </c>
       <c r="L17" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforePostSourceDocumentEvent '</v>
+        <v>When 'Trigger CheckLookupvalueExistsOnSalesHeader Whse. Posting'</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1567,7 +1562,7 @@
       </c>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1573,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="20" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="21"/>
@@ -1587,15 +1582,15 @@
       </c>
       <c r="J20" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0104] Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</v>
+        <v>[SCENARIO #0104] Check InheritLookupValueFromCustomer</v>
       </c>
       <c r="K20" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0104] Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber</v>
+        <v>//[SCENARIO #0104] Check InheritLookupValueFromCustomer</v>
       </c>
       <c r="L20" s="29" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0104 'Check OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent subscriber' {</v>
+        <v>Scenario 0104 'Check InheritLookupValueFromCustomer' {</v>
       </c>
       <c r="M20" s="21"/>
     </row>
@@ -1657,7 +1652,7 @@
         <v>Given 'Sales header without lookup value'</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1668,22 +1663,22 @@
         <v>14</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I23" s="25">
         <v>104</v>
       </c>
       <c r="J23" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </v>
+        <v>[WHEN] Trigger InheritLookupValueFromCustomer</v>
       </c>
       <c r="K23" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent </v>
+        <v>//[WHEN] Trigger InheritLookupValueFromCustomer</v>
       </c>
       <c r="L23" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnAfterCopySellToCustomerAddressFieldsFromCustomerEvent '</v>
+        <v>When 'Trigger InheritLookupValueFromCustomer'</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1715,7 +1710,7 @@
         <v>Then 'Lookup value on sales document is populated with lookup value of customer' }</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>11</v>
       </c>
@@ -1726,7 +1721,7 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="20" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="21"/>
@@ -1735,15 +1730,15 @@
       </c>
       <c r="J25" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0105] Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</v>
+        <v>[SCENARIO #0105] Check ApplyLookupValueFromCustomerTemplate from Contact</v>
       </c>
       <c r="K25" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0105] Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber</v>
+        <v>//[SCENARIO #0105] Check ApplyLookupValueFromCustomerTemplate from Contact</v>
       </c>
       <c r="L25" s="29" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0105 'Check OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent subscriber' {</v>
+        <v>Scenario 0105 'Check ApplyLookupValueFromCustomerTemplate from Contact' {</v>
       </c>
       <c r="M25" s="21"/>
     </row>
@@ -1805,7 +1800,7 @@
         <v>Given 'Customer'</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1816,22 +1811,22 @@
         <v>14</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I28" s="13">
         <v>105</v>
       </c>
       <c r="J28" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </v>
+        <v>[WHEN] Trigger ApplyLookupValueFromCustomerTemplate</v>
       </c>
       <c r="K28" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent </v>
+        <v>//[WHEN] Trigger ApplyLookupValueFromCustomerTemplate</v>
       </c>
       <c r="L28" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnCreateCustomerFromTemplateOnBeforeCustomerInsertEvent '</v>
+        <v>When 'Trigger ApplyLookupValueFromCustomerTemplate'</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1863,7 +1858,7 @@
         <v>Then 'Lookup value on customer is populated with lookup value of customer template' }</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>11</v>
       </c>
@@ -1874,7 +1869,7 @@
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="20" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="21"/>
@@ -1883,15 +1878,15 @@
       </c>
       <c r="J30" s="23" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0106] Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</v>
+        <v>[SCENARIO #0106] Check ApplyLookupValueFromCustomerTemplate</v>
       </c>
       <c r="K30" s="24" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0106] Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber</v>
+        <v>//[SCENARIO #0106] Check ApplyLookupValueFromCustomerTemplate</v>
       </c>
       <c r="L30" s="29" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0106 'Check OnApplyTemplateOnBeforeCustomerModifyEvent subscriber' {</v>
+        <v>Scenario 0106 'Check ApplyLookupValueFromCustomerTemplate' {</v>
       </c>
       <c r="M30" s="21"/>
     </row>
@@ -1964,22 +1959,22 @@
         <v>14</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I33" s="13">
         <v>106</v>
       </c>
       <c r="J33" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnApplyTemplateOnBeforeCustomerModifyEvent </v>
+        <v>[WHEN] Trigger ApplyLookupValueFromCustomerTemplate</v>
       </c>
       <c r="K33" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnApplyTemplateOnBeforeCustomerModifyEvent </v>
+        <v>//[WHEN] Trigger ApplyLookupValueFromCustomerTemplate</v>
       </c>
       <c r="L33" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnApplyTemplateOnBeforeCustomerModifyEvent '</v>
+        <v>When 'Trigger ApplyLookupValueFromCustomerTemplate'</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2041,7 +2036,7 @@
       </c>
       <c r="M35" s="8"/>
     </row>
-    <row r="36" spans="1:13" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>11</v>
       </c>
@@ -2052,7 +2047,7 @@
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G36" s="32"/>
       <c r="H36" s="35"/>
@@ -2061,15 +2056,15 @@
       </c>
       <c r="J36" s="37" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
+        <v>[SCENARIO #0107] Check InheritLookupValueFromSalesHeader</v>
       </c>
       <c r="K36" s="38" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0107] Check OnBeforeCreateShptLineFromSalesLineEvent subscriber</v>
+        <v>//[SCENARIO #0107] Check InheritLookupValueFromSalesHeader</v>
       </c>
       <c r="L36" s="39" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0107 'Check OnBeforeCreateShptLineFromSalesLineEvent subscriber' {</v>
+        <v>Scenario 0107 'Check InheritLookupValueFromSalesHeader' {</v>
       </c>
       <c r="M36" s="35"/>
     </row>
@@ -2084,7 +2079,7 @@
         <v>13</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I37" s="13">
         <v>107</v>
@@ -2113,7 +2108,7 @@
         <v>13</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I38" s="13">
         <v>107</v>
@@ -2142,22 +2137,22 @@
         <v>14</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I39" s="13">
         <v>107</v>
       </c>
       <c r="J39" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
+        <v>[WHEN] Trigger InheritLookupValueFromSalesHeader</v>
       </c>
       <c r="K39" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[WHEN] OnBeforeCreateShptLineFromSalesLineEvent </v>
+        <v>//[WHEN] Trigger InheritLookupValueFromSalesHeader</v>
       </c>
       <c r="L39" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'OnBeforeCreateShptLineFromSalesLineEvent '</v>
+        <v>When 'Trigger InheritLookupValueFromSalesHeader'</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2171,7 +2166,7 @@
         <v>15</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I40" s="13">
         <v>107</v>

</xml_diff>

<commit_message>
Removed duplicate scenario 107 and obsolete 106
</commit_message>
<xml_diff>
--- a/Excel sheets/ATDD Scenarios/LookupValue - Chapter 12.xlsx
+++ b/Excel sheets/ATDD Scenarios/LookupValue - Chapter 12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0699A838-20D2-4642-92A9-DB7326D1B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C54135-0BD3-484B-B4B6-95D1DA84CD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
   <si>
     <t>Feature</t>
   </si>
@@ -129,9 +129,6 @@
     <t>No error thrown</t>
   </si>
   <si>
-    <t>Inheritance - Customer Templates</t>
-  </si>
-  <si>
     <t>Lookup value on customer is populated with lookup value of customer template</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
   </si>
   <si>
     <t>Trigger ApplyLookupValueFromCustomerTemplate</t>
-  </si>
-  <si>
-    <t>Check ApplyLookupValueFromCustomerTemplate</t>
   </si>
   <si>
     <t>Check ApplyLookupValueFromCustomerTemplate from Contact</t>
@@ -403,69 +397,6 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -561,6 +492,69 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -575,28 +569,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M40" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:M40" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:M35" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A1:M35" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
     <tableColumn id="11" xr3:uid="{8F685D88-2001-49B6-A560-44AC61A85751}" name="Document"/>
-    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{4B57D4E1-7F53-4AB1-93B7-628D0D759AD9}" name="UI" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{3B45BC65-AA1D-4611-BFDF-489E623921CC}" name="Positive-negative" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{2B877830-769C-4915-8F5E-FA01A5B40D0A}" name="Scenario" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{470B84A4-8789-448A-A9D4-722FDC7901C1}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{187F9A26-F5CB-459C-8492-DB888AAB8AB0}" name="Given-When-Then (Description)" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{4877F37D-5FB5-43A6-8EB2-58971E92F829}" name="Scenario #" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{FB203AB3-EB4E-44B7-8CE3-8DC29CEF57D6}" name="ATDD Format" dataDxfId="15">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{C2A0C887-D273-4FD4-A6E5-600431087352}" name="Code Format" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{36DC9E15-3976-4F56-8FA0-7CF688CBA94D}" name="ATDD.TestScriptor Format" dataDxfId="13">
       <calculatedColumnFormula>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4AFC5B46-7C66-43E4-9E10-A3B6652FAF25}" name="Notes" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -899,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -1005,7 +999,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="21"/>
@@ -1043,7 +1037,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="13">
         <v>100</v>
@@ -1061,7 +1055,7 @@
         <v>Given 'Sales header without lookup value'</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1072,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I5" s="13">
         <v>100</v>
@@ -1113,7 +1107,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="13">
         <v>100</v>
@@ -1144,7 +1138,7 @@
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="21"/>
@@ -1179,7 +1173,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" s="13">
         <v>101</v>
@@ -1197,7 +1191,7 @@
         <v>Given 'Sales header with lookup value'</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1211,7 +1205,7 @@
         <v>14</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I9" s="13">
         <v>101</v>
@@ -1276,7 +1270,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="21"/>
@@ -1314,7 +1308,7 @@
         <v>13</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" s="13">
         <v>102</v>
@@ -1332,7 +1326,7 @@
         <v>Given 'Sales header with number and without lookup value'</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1349,7 +1343,7 @@
         <v>14</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I13" s="13">
         <v>102</v>
@@ -1384,7 +1378,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="13">
         <v>102</v>
@@ -1415,7 +1409,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="21"/>
@@ -1450,7 +1444,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="13">
         <v>103</v>
@@ -1468,7 +1462,7 @@
         <v>Given 'Sales header with number and lookup value'</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1482,7 +1476,7 @@
         <v>14</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I17" s="13">
         <v>103</v>
@@ -1573,7 +1567,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="21"/>
@@ -1634,7 +1628,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="25">
         <v>104</v>
@@ -1663,7 +1657,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I23" s="25">
         <v>104</v>
@@ -1710,7 +1704,7 @@
         <v>Then 'Lookup value on sales document is populated with lookup value of customer' }</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>11</v>
       </c>
@@ -1721,7 +1715,7 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="21"/>
@@ -1811,7 +1805,7 @@
         <v>14</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="13">
         <v>105</v>
@@ -1829,7 +1823,7 @@
         <v>When 'Trigger ApplyLookupValueFromCustomerTemplate'</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1840,7 +1834,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I29" s="13">
         <v>105</v>
@@ -1855,338 +1849,190 @@
       </c>
       <c r="L29" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on customer is populated with lookup value of customer template' }</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="22">
-        <v>106</v>
-      </c>
-      <c r="J30" s="23" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0106] Check ApplyLookupValueFromCustomerTemplate</v>
-      </c>
-      <c r="K30" s="24" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0106] Check ApplyLookupValueFromCustomerTemplate</v>
-      </c>
-      <c r="L30" s="29" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0106 'Check ApplyLookupValueFromCustomerTemplate' {</v>
-      </c>
-      <c r="M30" s="21"/>
-    </row>
-    <row r="31" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I31" s="13">
-        <v>106</v>
-      </c>
-      <c r="J31" s="14" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="K31" s="15" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer template with lookup value</v>
-      </c>
-      <c r="L31" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer template with lookup value'</v>
-      </c>
+        <v>Then 'Lookup value on customer is populated with lookup value of customer template' } }</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="16" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] LookupValue UT Warehouse Shipment</v>
+      </c>
+      <c r="K30" s="17" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] LookupValue UT Warehouse Shipment</v>
+      </c>
+      <c r="L30" s="28" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'LookupValue UT Warehouse Shipment' {</v>
+      </c>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="32"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="36">
+        <v>107</v>
+      </c>
+      <c r="J31" s="37" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0107] Check InheritLookupValueFromSalesHeader</v>
+      </c>
+      <c r="K31" s="38" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0107] Check InheritLookupValueFromSalesHeader</v>
+      </c>
+      <c r="L31" s="39" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0107 'Check InheritLookupValueFromSalesHeader' {</v>
+      </c>
+      <c r="M31" s="35"/>
     </row>
     <row r="32" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G32" t="s">
         <v>13</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="I32" s="13">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J32" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer</v>
+        <v>[GIVEN] Sales header with lookup value</v>
       </c>
       <c r="K32" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer</v>
+        <v>//[GIVEN] Sales header with lookup value</v>
       </c>
       <c r="L32" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer'</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Sales header with lookup value'</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" s="13">
+        <v>107</v>
+      </c>
+      <c r="J33" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Warehouse shipment line</v>
+      </c>
+      <c r="K33" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Warehouse shipment line</v>
+      </c>
+      <c r="L33" s="27" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Warehouse shipment line'</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I33" s="13">
-        <v>106</v>
-      </c>
-      <c r="J33" s="14" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Trigger ApplyLookupValueFromCustomerTemplate</v>
-      </c>
-      <c r="K33" s="15" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Trigger ApplyLookupValueFromCustomerTemplate</v>
-      </c>
-      <c r="L33" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Trigger ApplyLookupValueFromCustomerTemplate'</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="H34" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="13">
+        <v>107</v>
+      </c>
+      <c r="J34" s="14" t="str">
+        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Trigger InheritLookupValueFromSalesHeader</v>
+      </c>
+      <c r="K34" s="15" t="str">
+        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Trigger InheritLookupValueFromSalesHeader</v>
+      </c>
+      <c r="L34" s="27" t="str">
+        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Trigger InheritLookupValueFromSalesHeader'</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I34" s="13">
-        <v>106</v>
-      </c>
-      <c r="J34" s="14" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Lookup value on customer is populated with lookup value of customer template</v>
-      </c>
-      <c r="K34" s="15" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Lookup value on customer is populated with lookup value of customer template</v>
-      </c>
-      <c r="L34" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Lookup value on customer is populated with lookup value of customer template' } }</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="16.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="16" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] LookupValue UT Warehouse Shipment</v>
-      </c>
-      <c r="K35" s="17" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] LookupValue UT Warehouse Shipment</v>
-      </c>
-      <c r="L35" s="28" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'LookupValue UT Warehouse Shipment' {</v>
-      </c>
-      <c r="M35" s="8"/>
-    </row>
-    <row r="36" spans="1:13" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G36" s="32"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="36">
+      <c r="H35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35" s="13">
         <v>107</v>
       </c>
-      <c r="J36" s="37" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0107] Check InheritLookupValueFromSalesHeader</v>
-      </c>
-      <c r="K36" s="38" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0107] Check InheritLookupValueFromSalesHeader</v>
-      </c>
-      <c r="L36" s="39" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0107 'Check InheritLookupValueFromSalesHeader' {</v>
-      </c>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I37" s="13">
-        <v>107</v>
-      </c>
-      <c r="J37" s="14" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="K37" s="15" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Sales header with lookup value</v>
-      </c>
-      <c r="L37" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Sales header with lookup value'</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" t="s">
-        <v>29</v>
-      </c>
-      <c r="G38" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I38" s="13">
-        <v>107</v>
-      </c>
-      <c r="J38" s="14" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Warehouse shipment line</v>
-      </c>
-      <c r="K38" s="15" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Warehouse shipment line</v>
-      </c>
-      <c r="L38" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Warehouse shipment line'</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>11</v>
-      </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="G39" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I39" s="13">
-        <v>107</v>
-      </c>
-      <c r="J39" s="14" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Trigger InheritLookupValueFromSalesHeader</v>
-      </c>
-      <c r="K39" s="15" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Trigger InheritLookupValueFromSalesHeader</v>
-      </c>
-      <c r="L39" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Trigger InheritLookupValueFromSalesHeader'</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="G40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I40" s="13">
-        <v>107</v>
-      </c>
-      <c r="J40" s="14" t="str">
+      <c r="J35" s="14" t="str">
         <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
       </c>
-      <c r="K40" s="15" t="str">
+      <c r="K35" s="15" t="str">
         <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Lookup value on warehouse shipment line is populated with lookup value of sales header</v>
       </c>
-      <c r="L40" s="27" t="str">
+      <c r="L35" s="27" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("G" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Lookup value on warehouse shipment line is populated with lookup value of sales header' } }</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:12" ht="15.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="I36:I1048576 I1:I34">
+  <conditionalFormatting sqref="I31:I1048576 I1:I29">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -2198,33 +2044,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:D1048576 D1:D34">
-    <cfRule type="cellIs" dxfId="21" priority="51" operator="equal">
+  <conditionalFormatting sqref="D31:D1048576 D1:D29">
+    <cfRule type="cellIs" dxfId="11" priority="51" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36:B1048576 A1:B34">
-    <cfRule type="containsBlanks" dxfId="20" priority="50">
+  <conditionalFormatting sqref="A31:B1048576 A1:B29">
+    <cfRule type="containsBlanks" dxfId="10" priority="50">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36:E1048576 E1:E34">
-    <cfRule type="cellIs" dxfId="19" priority="46" operator="equal">
+  <conditionalFormatting sqref="E31:E1048576 E1:E29">
+    <cfRule type="cellIs" dxfId="9" priority="46" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G36:G1048576 G1:G34">
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+  <conditionalFormatting sqref="G31:G1048576 G1:G29">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
+  <conditionalFormatting sqref="I30">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2236,29 +2082,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+  <conditionalFormatting sqref="D30">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35:B35">
-    <cfRule type="containsBlanks" dxfId="14" priority="5">
-      <formula>LEN(TRIM(A35))=0</formula>
+  <conditionalFormatting sqref="A30:B30">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(A30))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+  <conditionalFormatting sqref="G30">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>